<commit_message>
Corrected inconsistent sample naming in test data
</commit_message>
<xml_diff>
--- a/data-raw/testdata/Rinder_labels.xlsx
+++ b/data-raw/testdata/Rinder_labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\HolomicsShiny\data-raw\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\Holomics\data-raw\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93FBDB7C-500F-462C-B050-C9D463D4569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC282BD-D9B9-42C1-A286-0EBA3D8A06EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A69F4C6-B362-4230-9AE0-DE87BA2683B7}"/>
   </bookViews>
@@ -261,9 +261,6 @@
     <t>L-V10-SuPhy2-d11-0h-R2</t>
   </si>
   <si>
-    <t>Rf-cows-pooled-d0-R3</t>
-  </si>
-  <si>
     <t>RF-Cows pooled</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t>L-V8-StPhy2-d10-8h-R2</t>
   </si>
   <si>
-    <t>Rf-cows-pooled-d0-R2</t>
-  </si>
-  <si>
     <t>L-V2-SuPhy2-d10-8h-R1</t>
   </si>
   <si>
@@ -372,9 +366,6 @@
     <t>L-V9-SuCon-d11-0h-R2</t>
   </si>
   <si>
-    <t>Rf-cows-pooled-d0-R1</t>
-  </si>
-  <si>
     <t>L-V8-TGSPhy2-d10-8h-R1</t>
   </si>
   <si>
@@ -403,6 +394,15 @@
   </si>
   <si>
     <t>L-V1-TGSCon-d11-0h-R2</t>
+  </si>
+  <si>
+    <t>RF-Cows-pooled-d0-R3</t>
+  </si>
+  <si>
+    <t>RF-Cows-pooled-d0-R2</t>
+  </si>
+  <si>
+    <t>RF-Cows-pooled-d0-R1</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE56592-BC49-4050-81FB-27B621FA07B6}">
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,15 +1294,15 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>33</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>27</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>17</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>33</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>9</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>33</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>27</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>27</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>15</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>9</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>17</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>9</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>13</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>15</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>5</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>15</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>27</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>7</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>7</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>13</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>13</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>15</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>9</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>33</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>15</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>3</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>3</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>7</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>9</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>5</v>
@@ -1550,15 +1550,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>17</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>33</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>13</v>
@@ -1582,15 +1582,15 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>7</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>13</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>7</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>27</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>9</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>27</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>15</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>13</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Samplenames are now identical
</commit_message>
<xml_diff>
--- a/data-raw/testdata/Rinder_labels.xlsx
+++ b/data-raw/testdata/Rinder_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\Holomics\data-raw\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC282BD-D9B9-42C1-A286-0EBA3D8A06EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB9357-B563-4B67-B4ED-6A6BFE5B0209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A69F4C6-B362-4230-9AE0-DE87BA2683B7}"/>
   </bookViews>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE56592-BC49-4050-81FB-27B621FA07B6}">
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>